<commit_message>
update hardware CAD & laser cut files
</commit_message>
<xml_diff>
--- a/MykroscopeHardware/Mykroscope BOM.xlsx
+++ b/MykroscopeHardware/Mykroscope BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisooi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Louis/Desktop/Mykroscope_Public/MykroscopeHardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E6A2652-2CB7-2249-B0A0-DACF8D212451}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AAE687-F8C8-AA43-9738-1A2C279F2253}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19220" xr2:uid="{8540E5CE-B374-6748-B855-3123FE1779AE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{8540E5CE-B374-6748-B855-3123FE1779AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Cardboard</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/LED-lamp-beads-lens-CREE-XPE-5050-5050-special-lens-25-degrees/32239378662.html?spm=a2g0s.13010208.99999999.262.OkeFEy</t>
-  </si>
-  <si>
     <t>Url</t>
   </si>
   <si>
@@ -73,13 +70,19 @@
   </si>
   <si>
     <t>https://item.taobao.com/item.htm?spm=a1z09.2.0.0.3b122e8diSsDmn&amp;id=564436847258&amp;_u=a35cq5ru044a</t>
+  </si>
+  <si>
+    <t>https://www.alibaba.com/product-detail/1mm-1-5mm-2mm-4mm-12mm_60275500727.html?spm=a2700.8443308.0.0.4b7a3e5fd82dtX</t>
+  </si>
+  <si>
+    <t>Lens Holder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,6 +94,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,18 +130,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,7 +460,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,7 +478,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -483,7 +497,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -494,12 +508,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -513,18 +527,18 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -534,23 +548,28 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>6</v>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
@@ -574,6 +593,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{E6C3CA09-6A46-1F44-B086-CE3970A7DC3F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>